<commit_message>
3 column tpl file for exp R006
</commit_message>
<xml_diff>
--- a/inst/dataInst/R006_TPL_Export_Int.xlsx
+++ b/inst/dataInst/R006_TPL_Export_Int.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="131">
   <si>
     <t>Sample Name (used in ZeptoView 3.1)</t>
   </si>
@@ -217,13 +217,208 @@
   </si>
   <si>
     <t>S064_cell line_Cell line mix_cell line mix____1_1</t>
+  </si>
+  <si>
+    <t>Zeptosens Sample ID</t>
+  </si>
+  <si>
+    <t>Sample#1</t>
+  </si>
+  <si>
+    <t>Sample#2</t>
+  </si>
+  <si>
+    <t>Sample#3</t>
+  </si>
+  <si>
+    <t>Sample#4</t>
+  </si>
+  <si>
+    <t>Sample#5</t>
+  </si>
+  <si>
+    <t>Sample#6</t>
+  </si>
+  <si>
+    <t>Sample#7</t>
+  </si>
+  <si>
+    <t>Sample#8</t>
+  </si>
+  <si>
+    <t>Sample#9</t>
+  </si>
+  <si>
+    <t>Sample#10</t>
+  </si>
+  <si>
+    <t>Sample#11</t>
+  </si>
+  <si>
+    <t>Sample#12</t>
+  </si>
+  <si>
+    <t>Sample#13</t>
+  </si>
+  <si>
+    <t>Sample#14</t>
+  </si>
+  <si>
+    <t>Sample#15</t>
+  </si>
+  <si>
+    <t>Sample#16</t>
+  </si>
+  <si>
+    <t>Sample#17</t>
+  </si>
+  <si>
+    <t>Sample#18</t>
+  </si>
+  <si>
+    <t>Sample#19</t>
+  </si>
+  <si>
+    <t>Sample#20</t>
+  </si>
+  <si>
+    <t>Sample#21</t>
+  </si>
+  <si>
+    <t>Sample#22</t>
+  </si>
+  <si>
+    <t>Sample#23</t>
+  </si>
+  <si>
+    <t>Sample#24</t>
+  </si>
+  <si>
+    <t>Sample#25</t>
+  </si>
+  <si>
+    <t>Sample#26</t>
+  </si>
+  <si>
+    <t>Sample#27</t>
+  </si>
+  <si>
+    <t>Sample#28</t>
+  </si>
+  <si>
+    <t>Sample#29</t>
+  </si>
+  <si>
+    <t>Sample#30</t>
+  </si>
+  <si>
+    <t>Sample#31</t>
+  </si>
+  <si>
+    <t>Sample#32</t>
+  </si>
+  <si>
+    <t>Sample#33</t>
+  </si>
+  <si>
+    <t>Sample#34</t>
+  </si>
+  <si>
+    <t>Sample#35</t>
+  </si>
+  <si>
+    <t>Sample#36</t>
+  </si>
+  <si>
+    <t>Sample#37</t>
+  </si>
+  <si>
+    <t>Sample#38</t>
+  </si>
+  <si>
+    <t>Sample#39</t>
+  </si>
+  <si>
+    <t>Sample#40</t>
+  </si>
+  <si>
+    <t>Sample#41</t>
+  </si>
+  <si>
+    <t>Sample#42</t>
+  </si>
+  <si>
+    <t>Sample#43</t>
+  </si>
+  <si>
+    <t>Sample#44</t>
+  </si>
+  <si>
+    <t>Sample#45</t>
+  </si>
+  <si>
+    <t>Sample#46</t>
+  </si>
+  <si>
+    <t>Sample#47</t>
+  </si>
+  <si>
+    <t>Sample#48</t>
+  </si>
+  <si>
+    <t>Sample#49</t>
+  </si>
+  <si>
+    <t>Sample#50</t>
+  </si>
+  <si>
+    <t>Sample#51</t>
+  </si>
+  <si>
+    <t>Sample#52</t>
+  </si>
+  <si>
+    <t>Sample#53</t>
+  </si>
+  <si>
+    <t>Sample#54</t>
+  </si>
+  <si>
+    <t>Sample#55</t>
+  </si>
+  <si>
+    <t>Sample#56</t>
+  </si>
+  <si>
+    <t>Sample#57</t>
+  </si>
+  <si>
+    <t>Sample#58</t>
+  </si>
+  <si>
+    <t>Sample#59</t>
+  </si>
+  <si>
+    <t>Sample#60</t>
+  </si>
+  <si>
+    <t>Sample#61</t>
+  </si>
+  <si>
+    <t>Sample#62</t>
+  </si>
+  <si>
+    <t>Sample#63</t>
+  </si>
+  <si>
+    <t>Sample#64</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -262,6 +457,21 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -283,7 +493,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -308,6 +518,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -640,903 +859,1093 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B157"/>
+  <dimension ref="A1:C156"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="77.6640625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="8"/>
+    <col min="1" max="1" width="10.83203125" style="11"/>
+    <col min="2" max="2" width="77.6640625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="84">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" ht="84">
+      <c r="A1" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:3">
+      <c r="A2" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4">
+      <c r="C2" s="4">
         <v>3.117</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:3">
+      <c r="A3" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4">
+      <c r="C3" s="4">
         <v>2.863</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:3">
+      <c r="A4" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="4">
+      <c r="C4" s="4">
         <v>2.524</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:3">
+      <c r="A5" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="4">
+      <c r="C5" s="4">
         <v>2.7669999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:3">
+      <c r="A6" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="4">
+      <c r="C6" s="4">
         <v>2.9289999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:3">
+      <c r="A7" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="4">
+      <c r="C7" s="4">
         <v>2.5819999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:3">
+      <c r="A8" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="4">
+      <c r="C8" s="4">
         <v>2.3170000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:3">
+      <c r="A9" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="4">
+      <c r="C9" s="4">
         <v>2.0640000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="5" t="s">
+    <row r="10" spans="1:3">
+      <c r="A10" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="4">
+      <c r="C10" s="4">
         <v>2.9319999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="5" t="s">
+    <row r="11" spans="1:3">
+      <c r="A11" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="4">
+      <c r="C11" s="4">
         <v>2.9969999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="5" t="s">
+    <row r="12" spans="1:3">
+      <c r="A12" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="4">
+      <c r="C12" s="4">
         <v>3.2210000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="5" t="s">
+    <row r="13" spans="1:3">
+      <c r="A13" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="4">
+      <c r="C13" s="4">
         <v>3.633</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="5" t="s">
+    <row r="14" spans="1:3">
+      <c r="A14" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="4">
+      <c r="C14" s="4">
         <v>3.1059999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="5" t="s">
+    <row r="15" spans="1:3">
+      <c r="A15" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="4">
+      <c r="C15" s="4">
         <v>2.976</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="5" t="s">
+    <row r="16" spans="1:3">
+      <c r="A16" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="4">
+      <c r="C16" s="4">
         <v>3.33</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="5" t="s">
+    <row r="17" spans="1:3">
+      <c r="A17" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="4">
+      <c r="C17" s="4">
         <v>3.4039999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="5" t="s">
+    <row r="18" spans="1:3">
+      <c r="A18" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="4">
+      <c r="C18" s="4">
         <v>3.2229999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="5" t="s">
+    <row r="19" spans="1:3">
+      <c r="A19" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="4">
+      <c r="C19" s="4">
         <v>2.87</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="5" t="s">
+    <row r="20" spans="1:3">
+      <c r="A20" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="4">
+      <c r="C20" s="4">
         <v>2.6970000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="5" t="s">
+    <row r="21" spans="1:3">
+      <c r="A21" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="4">
+      <c r="C21" s="4">
         <v>2.6680000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="5" t="s">
+    <row r="22" spans="1:3">
+      <c r="A22" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="4">
+      <c r="C22" s="4">
         <v>3.2080000000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="5" t="s">
+    <row r="23" spans="1:3">
+      <c r="A23" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="4">
+      <c r="C23" s="4">
         <v>2.9630000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="5" t="s">
+    <row r="24" spans="1:3">
+      <c r="A24" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="4">
+      <c r="C24" s="4">
         <v>2.7989999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="5" t="s">
+    <row r="25" spans="1:3">
+      <c r="A25" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="4">
+      <c r="C25" s="4">
         <v>3.6459999999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="5" t="s">
+    <row r="26" spans="1:3">
+      <c r="A26" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="6">
+      <c r="C26" s="6">
         <v>3.2949999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="5" t="s">
+    <row r="27" spans="1:3">
+      <c r="A27" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="6">
+      <c r="C27" s="6">
         <v>3.2709999999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="5" t="s">
+    <row r="28" spans="1:3">
+      <c r="A28" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="6">
+      <c r="C28" s="6">
         <v>3.2440000000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="5" t="s">
+    <row r="29" spans="1:3">
+      <c r="A29" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="6">
+      <c r="C29" s="6">
         <v>3.3330000000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="5" t="s">
+    <row r="30" spans="1:3">
+      <c r="A30" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="6">
+      <c r="C30" s="6">
         <v>3.073</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="5" t="s">
+    <row r="31" spans="1:3">
+      <c r="A31" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="6">
+      <c r="C31" s="6">
         <v>2.298</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="5" t="s">
+    <row r="32" spans="1:3">
+      <c r="A32" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="6">
+      <c r="C32" s="6">
         <v>2.4809999999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="5" t="s">
+    <row r="33" spans="1:3">
+      <c r="A33" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="6">
+      <c r="C33" s="6">
         <v>2.8330000000000002</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="5" t="s">
+    <row r="34" spans="1:3">
+      <c r="A34" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="6">
+      <c r="C34" s="6">
         <v>2.6930000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="5" t="s">
+    <row r="35" spans="1:3">
+      <c r="A35" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="6">
+      <c r="C35" s="6">
         <v>2.8570000000000002</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="5" t="s">
+    <row r="36" spans="1:3">
+      <c r="A36" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="6">
+      <c r="C36" s="6">
         <v>3.05</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="5" t="s">
+    <row r="37" spans="1:3">
+      <c r="A37" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="6">
+      <c r="C37" s="6">
         <v>3.1379999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="5" t="s">
+    <row r="38" spans="1:3">
+      <c r="A38" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="6">
+      <c r="C38" s="6">
         <v>3.1539999999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="5" t="s">
+    <row r="39" spans="1:3">
+      <c r="A39" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="6">
+      <c r="C39" s="6">
         <v>2.9620000000000002</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="5" t="s">
+    <row r="40" spans="1:3">
+      <c r="A40" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="6">
+      <c r="C40" s="6">
         <v>3.173</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="5" t="s">
+    <row r="41" spans="1:3">
+      <c r="A41" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B41" s="6">
+      <c r="C41" s="6">
         <v>3.0369999999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
-      <c r="A42" s="5" t="s">
+    <row r="42" spans="1:3">
+      <c r="A42" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B42" s="6">
+      <c r="C42" s="6">
         <v>3.0110000000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
-      <c r="A43" s="5" t="s">
+    <row r="43" spans="1:3">
+      <c r="A43" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B43" s="6">
+      <c r="C43" s="6">
         <v>2.379</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
-      <c r="A44" s="5" t="s">
+    <row r="44" spans="1:3">
+      <c r="A44" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B44" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B44" s="6">
+      <c r="C44" s="6">
         <v>2.532</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
-      <c r="A45" s="5" t="s">
+    <row r="45" spans="1:3">
+      <c r="A45" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B45" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B45" s="6">
+      <c r="C45" s="6">
         <v>2.5649999999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
-      <c r="A46" s="5" t="s">
+    <row r="46" spans="1:3">
+      <c r="A46" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B46" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B46" s="6">
+      <c r="C46" s="6">
         <v>3.8149999999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
-      <c r="A47" s="5" t="s">
+    <row r="47" spans="1:3">
+      <c r="A47" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B47" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B47" s="6">
+      <c r="C47" s="6">
         <v>3.6030000000000002</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
-      <c r="A48" s="5" t="s">
+    <row r="48" spans="1:3">
+      <c r="A48" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B48" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B48" s="6">
+      <c r="C48" s="6">
         <v>3.3940000000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="5" t="s">
+    <row r="49" spans="1:3">
+      <c r="A49" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B49" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B49" s="6">
+      <c r="C49" s="6">
         <v>4.0640000000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
-      <c r="A50" s="5" t="s">
+    <row r="50" spans="1:3">
+      <c r="A50" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B50" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B50" s="6">
+      <c r="C50" s="6">
         <v>3.4409999999999998</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
-      <c r="A51" s="5" t="s">
+    <row r="51" spans="1:3">
+      <c r="A51" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B51" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B51" s="6">
+      <c r="C51" s="6">
         <v>3.0339999999999998</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
-      <c r="A52" s="5" t="s">
+    <row r="52" spans="1:3">
+      <c r="A52" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B52" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B52" s="6">
+      <c r="C52" s="6">
         <v>2.1859999999999999</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
-      <c r="A53" s="5" t="s">
+    <row r="53" spans="1:3">
+      <c r="A53" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B53" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B53" s="6">
+      <c r="C53" s="6">
         <v>5.0069999999999997</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
-      <c r="A54" s="5" t="s">
+    <row r="54" spans="1:3">
+      <c r="A54" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B54" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B54" s="6">
+      <c r="C54" s="6">
         <v>3.9249999999999998</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
-      <c r="A55" s="5" t="s">
+    <row r="55" spans="1:3">
+      <c r="A55" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B55" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B55" s="6">
+      <c r="C55" s="6">
         <v>3.1520000000000001</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
-      <c r="A56" s="5" t="s">
+    <row r="56" spans="1:3">
+      <c r="A56" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B56" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B56" s="6">
+      <c r="C56" s="6">
         <v>4.0229999999999997</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
-      <c r="A57" s="5" t="s">
+    <row r="57" spans="1:3">
+      <c r="A57" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B57" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B57" s="6">
+      <c r="C57" s="6">
         <v>3.6549999999999998</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
-      <c r="A58" s="5" t="s">
+    <row r="58" spans="1:3">
+      <c r="A58" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B58" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B58" s="6">
+      <c r="C58" s="6">
         <v>2.5750000000000002</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="5" t="s">
+    <row r="59" spans="1:3">
+      <c r="A59" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B59" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B59" s="6">
+      <c r="C59" s="6">
         <v>3.6840000000000002</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
-      <c r="A60" s="5" t="s">
+    <row r="60" spans="1:3">
+      <c r="A60" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B60" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B60" s="6">
+      <c r="C60" s="6">
         <v>2.2090000000000001</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
-      <c r="A61" s="5" t="s">
+    <row r="61" spans="1:3">
+      <c r="A61" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B61" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B61" s="6">
+      <c r="C61" s="6">
         <v>2.0720000000000001</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
-      <c r="A62" s="5" t="s">
+    <row r="62" spans="1:3">
+      <c r="A62" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="B62" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B62" s="6">
+      <c r="C62" s="6">
         <v>3.2330000000000001</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
-      <c r="A63" s="5" t="s">
+    <row r="63" spans="1:3">
+      <c r="A63" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="B63" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B63" s="6">
+      <c r="C63" s="6">
         <v>2.0369999999999999</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
-      <c r="A64" s="5" t="s">
+    <row r="64" spans="1:3">
+      <c r="A64" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B64" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B64" s="6">
+      <c r="C64" s="6">
         <v>1.347</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
-      <c r="A65" s="5" t="s">
+    <row r="65" spans="1:3">
+      <c r="A65" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B65" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B65" s="6"/>
-    </row>
-    <row r="66" spans="1:2">
-      <c r="A66" s="5"/>
-      <c r="B66" s="6"/>
-    </row>
-    <row r="67" spans="1:2">
-      <c r="A67" s="5"/>
-      <c r="B67" s="6"/>
-    </row>
-    <row r="68" spans="1:2">
-      <c r="A68" s="5"/>
-      <c r="B68" s="7"/>
-    </row>
-    <row r="69" spans="1:2">
-      <c r="A69" s="5"/>
-      <c r="B69" s="7"/>
-    </row>
-    <row r="70" spans="1:2">
-      <c r="A70" s="5"/>
-      <c r="B70" s="7"/>
-    </row>
-    <row r="71" spans="1:2">
-      <c r="A71" s="5"/>
-      <c r="B71" s="7"/>
-    </row>
-    <row r="72" spans="1:2">
-      <c r="A72" s="5"/>
-      <c r="B72" s="7"/>
-    </row>
-    <row r="73" spans="1:2">
-      <c r="A73" s="5"/>
-      <c r="B73" s="7"/>
-    </row>
-    <row r="74" spans="1:2">
-      <c r="A74" s="5"/>
-      <c r="B74" s="7"/>
-    </row>
-    <row r="75" spans="1:2">
-      <c r="A75" s="5"/>
-      <c r="B75" s="7"/>
-    </row>
-    <row r="76" spans="1:2">
-      <c r="A76" s="5"/>
-      <c r="B76" s="7"/>
-    </row>
-    <row r="77" spans="1:2">
-      <c r="A77" s="5"/>
-      <c r="B77" s="7"/>
-    </row>
-    <row r="78" spans="1:2">
-      <c r="A78" s="5"/>
-      <c r="B78" s="7"/>
-    </row>
-    <row r="79" spans="1:2">
-      <c r="A79" s="5"/>
-      <c r="B79" s="7"/>
-    </row>
-    <row r="80" spans="1:2">
-      <c r="A80" s="5"/>
-      <c r="B80" s="7"/>
-    </row>
-    <row r="81" spans="1:2">
-      <c r="A81" s="5"/>
-      <c r="B81" s="7"/>
-    </row>
-    <row r="82" spans="1:2">
-      <c r="A82" s="5"/>
-      <c r="B82" s="7"/>
-    </row>
-    <row r="83" spans="1:2">
-      <c r="A83" s="5"/>
-      <c r="B83" s="7"/>
-    </row>
-    <row r="84" spans="1:2">
-      <c r="A84" s="5"/>
-      <c r="B84" s="7"/>
-    </row>
-    <row r="85" spans="1:2">
-      <c r="A85" s="5"/>
-      <c r="B85" s="7"/>
-    </row>
-    <row r="86" spans="1:2">
-      <c r="A86" s="5"/>
-      <c r="B86" s="7"/>
-    </row>
-    <row r="87" spans="1:2">
-      <c r="A87" s="5"/>
-      <c r="B87" s="7"/>
-    </row>
-    <row r="88" spans="1:2">
-      <c r="A88" s="5"/>
-      <c r="B88" s="7"/>
-    </row>
-    <row r="89" spans="1:2">
-      <c r="A89" s="5"/>
-      <c r="B89" s="7"/>
-    </row>
-    <row r="90" spans="1:2">
-      <c r="A90" s="5"/>
-      <c r="B90" s="7"/>
-    </row>
-    <row r="91" spans="1:2">
-      <c r="A91" s="5"/>
-      <c r="B91" s="7"/>
-    </row>
-    <row r="92" spans="1:2">
-      <c r="A92" s="5"/>
-      <c r="B92" s="7"/>
-    </row>
-    <row r="93" spans="1:2">
-      <c r="A93" s="5"/>
-      <c r="B93" s="7"/>
-    </row>
-    <row r="94" spans="1:2">
-      <c r="A94" s="5"/>
-      <c r="B94" s="7"/>
-    </row>
-    <row r="95" spans="1:2">
-      <c r="A95" s="5"/>
-      <c r="B95" s="7"/>
-    </row>
-    <row r="96" spans="1:2">
-      <c r="A96" s="5"/>
-      <c r="B96" s="7"/>
-    </row>
-    <row r="97" spans="1:2">
-      <c r="A97" s="5"/>
-      <c r="B97" s="7"/>
-    </row>
-    <row r="98" spans="1:2">
-      <c r="A98" s="5"/>
+      <c r="C65" s="6"/>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="B66" s="5"/>
+      <c r="C66" s="6"/>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="B67" s="5"/>
+      <c r="C67" s="7"/>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="B68" s="5"/>
+      <c r="C68" s="7"/>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="B69" s="5"/>
+      <c r="C69" s="7"/>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="B70" s="5"/>
+      <c r="C70" s="7"/>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="B71" s="5"/>
+      <c r="C71" s="7"/>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="B72" s="5"/>
+      <c r="C72" s="7"/>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="B73" s="5"/>
+      <c r="C73" s="7"/>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="B74" s="5"/>
+      <c r="C74" s="7"/>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="B75" s="5"/>
+      <c r="C75" s="7"/>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="B76" s="5"/>
+      <c r="C76" s="7"/>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="B77" s="5"/>
+      <c r="C77" s="7"/>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="B78" s="5"/>
+      <c r="C78" s="7"/>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="B79" s="5"/>
+      <c r="C79" s="7"/>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="B80" s="5"/>
+      <c r="C80" s="7"/>
+    </row>
+    <row r="81" spans="2:3">
+      <c r="B81" s="5"/>
+      <c r="C81" s="7"/>
+    </row>
+    <row r="82" spans="2:3">
+      <c r="B82" s="5"/>
+      <c r="C82" s="7"/>
+    </row>
+    <row r="83" spans="2:3">
+      <c r="B83" s="5"/>
+      <c r="C83" s="7"/>
+    </row>
+    <row r="84" spans="2:3">
+      <c r="B84" s="5"/>
+      <c r="C84" s="7"/>
+    </row>
+    <row r="85" spans="2:3">
+      <c r="B85" s="5"/>
+      <c r="C85" s="7"/>
+    </row>
+    <row r="86" spans="2:3">
+      <c r="B86" s="5"/>
+      <c r="C86" s="7"/>
+    </row>
+    <row r="87" spans="2:3">
+      <c r="B87" s="5"/>
+      <c r="C87" s="7"/>
+    </row>
+    <row r="88" spans="2:3">
+      <c r="B88" s="5"/>
+      <c r="C88" s="7"/>
+    </row>
+    <row r="89" spans="2:3">
+      <c r="B89" s="5"/>
+      <c r="C89" s="7"/>
+    </row>
+    <row r="90" spans="2:3">
+      <c r="B90" s="5"/>
+      <c r="C90" s="7"/>
+    </row>
+    <row r="91" spans="2:3">
+      <c r="B91" s="5"/>
+      <c r="C91" s="7"/>
+    </row>
+    <row r="92" spans="2:3">
+      <c r="B92" s="5"/>
+      <c r="C92" s="7"/>
+    </row>
+    <row r="93" spans="2:3">
+      <c r="B93" s="5"/>
+      <c r="C93" s="7"/>
+    </row>
+    <row r="94" spans="2:3">
+      <c r="B94" s="5"/>
+      <c r="C94" s="7"/>
+    </row>
+    <row r="95" spans="2:3">
+      <c r="B95" s="5"/>
+      <c r="C95" s="7"/>
+    </row>
+    <row r="96" spans="2:3">
+      <c r="B96" s="5"/>
+      <c r="C96" s="7"/>
+    </row>
+    <row r="97" spans="2:3">
+      <c r="B97" s="5"/>
+      <c r="C97" s="5"/>
+    </row>
+    <row r="98" spans="2:3">
       <c r="B98" s="5"/>
-    </row>
-    <row r="99" spans="1:2">
-      <c r="A99" s="5"/>
+      <c r="C98" s="5"/>
+    </row>
+    <row r="99" spans="2:3">
       <c r="B99" s="5"/>
-    </row>
-    <row r="100" spans="1:2">
-      <c r="A100" s="5"/>
+      <c r="C99" s="5"/>
+    </row>
+    <row r="100" spans="2:3">
       <c r="B100" s="5"/>
-    </row>
-    <row r="101" spans="1:2">
-      <c r="A101" s="5"/>
+      <c r="C100" s="5"/>
+    </row>
+    <row r="101" spans="2:3">
       <c r="B101" s="5"/>
-    </row>
-    <row r="102" spans="1:2">
-      <c r="A102" s="5"/>
+      <c r="C101" s="5"/>
+    </row>
+    <row r="102" spans="2:3">
       <c r="B102" s="5"/>
-    </row>
-    <row r="103" spans="1:2">
-      <c r="A103" s="5"/>
+      <c r="C102" s="5"/>
+    </row>
+    <row r="103" spans="2:3">
       <c r="B103" s="5"/>
-    </row>
-    <row r="104" spans="1:2">
-      <c r="A104" s="5"/>
+      <c r="C103" s="5"/>
+    </row>
+    <row r="104" spans="2:3">
       <c r="B104" s="5"/>
-    </row>
-    <row r="105" spans="1:2">
-      <c r="A105" s="5"/>
+      <c r="C104" s="5"/>
+    </row>
+    <row r="105" spans="2:3">
       <c r="B105" s="5"/>
-    </row>
-    <row r="106" spans="1:2">
-      <c r="A106" s="5"/>
+      <c r="C105" s="5"/>
+    </row>
+    <row r="106" spans="2:3">
       <c r="B106" s="5"/>
-    </row>
-    <row r="107" spans="1:2">
-      <c r="A107" s="5"/>
+      <c r="C106" s="5"/>
+    </row>
+    <row r="107" spans="2:3">
       <c r="B107" s="5"/>
-    </row>
-    <row r="108" spans="1:2">
-      <c r="A108" s="5"/>
+      <c r="C107" s="5"/>
+    </row>
+    <row r="108" spans="2:3">
       <c r="B108" s="5"/>
-    </row>
-    <row r="109" spans="1:2">
-      <c r="A109" s="5"/>
+      <c r="C108" s="5"/>
+    </row>
+    <row r="109" spans="2:3">
       <c r="B109" s="5"/>
-    </row>
-    <row r="110" spans="1:2">
-      <c r="A110" s="5"/>
+      <c r="C109" s="5"/>
+    </row>
+    <row r="110" spans="2:3">
       <c r="B110" s="5"/>
-    </row>
-    <row r="111" spans="1:2">
-      <c r="A111" s="5"/>
+      <c r="C110" s="5"/>
+    </row>
+    <row r="111" spans="2:3">
       <c r="B111" s="5"/>
-    </row>
-    <row r="112" spans="1:2">
-      <c r="A112" s="5"/>
+      <c r="C111" s="5"/>
+    </row>
+    <row r="112" spans="2:3">
       <c r="B112" s="5"/>
-    </row>
-    <row r="113" spans="1:2">
-      <c r="A113" s="5"/>
+      <c r="C112" s="5"/>
+    </row>
+    <row r="113" spans="2:3">
       <c r="B113" s="5"/>
-    </row>
-    <row r="114" spans="1:2">
-      <c r="A114" s="5"/>
+      <c r="C113" s="5"/>
+    </row>
+    <row r="114" spans="2:3">
       <c r="B114" s="5"/>
-    </row>
-    <row r="115" spans="1:2">
-      <c r="A115" s="5"/>
+      <c r="C114" s="5"/>
+    </row>
+    <row r="115" spans="2:3">
       <c r="B115" s="5"/>
-    </row>
-    <row r="116" spans="1:2">
-      <c r="A116" s="5"/>
+      <c r="C115" s="5"/>
+    </row>
+    <row r="116" spans="2:3">
       <c r="B116" s="5"/>
-    </row>
-    <row r="117" spans="1:2">
-      <c r="A117" s="5"/>
+      <c r="C116" s="5"/>
+    </row>
+    <row r="117" spans="2:3">
       <c r="B117" s="5"/>
-    </row>
-    <row r="118" spans="1:2">
-      <c r="A118" s="5"/>
+      <c r="C117" s="5"/>
+    </row>
+    <row r="118" spans="2:3">
       <c r="B118" s="5"/>
-    </row>
-    <row r="119" spans="1:2">
-      <c r="A119" s="5"/>
+      <c r="C118" s="5"/>
+    </row>
+    <row r="119" spans="2:3">
       <c r="B119" s="5"/>
-    </row>
-    <row r="120" spans="1:2">
-      <c r="A120" s="5"/>
+      <c r="C119" s="5"/>
+    </row>
+    <row r="120" spans="2:3">
       <c r="B120" s="5"/>
-    </row>
-    <row r="121" spans="1:2">
-      <c r="A121" s="5"/>
+      <c r="C120" s="5"/>
+    </row>
+    <row r="121" spans="2:3">
       <c r="B121" s="5"/>
-    </row>
-    <row r="122" spans="1:2">
-      <c r="A122" s="5"/>
+      <c r="C121" s="5"/>
+    </row>
+    <row r="122" spans="2:3">
       <c r="B122" s="5"/>
-    </row>
-    <row r="123" spans="1:2">
-      <c r="A123" s="5"/>
+      <c r="C122" s="5"/>
+    </row>
+    <row r="123" spans="2:3">
       <c r="B123" s="5"/>
-    </row>
-    <row r="124" spans="1:2">
-      <c r="A124" s="5"/>
+      <c r="C123" s="5"/>
+    </row>
+    <row r="124" spans="2:3">
       <c r="B124" s="5"/>
-    </row>
-    <row r="125" spans="1:2">
-      <c r="A125" s="5"/>
+      <c r="C124" s="5"/>
+    </row>
+    <row r="125" spans="2:3">
       <c r="B125" s="5"/>
-    </row>
-    <row r="126" spans="1:2">
-      <c r="A126" s="5"/>
+      <c r="C125" s="5"/>
+    </row>
+    <row r="126" spans="2:3">
       <c r="B126" s="5"/>
-    </row>
-    <row r="127" spans="1:2">
-      <c r="A127" s="5"/>
+      <c r="C126" s="5"/>
+    </row>
+    <row r="127" spans="2:3">
       <c r="B127" s="5"/>
-    </row>
-    <row r="128" spans="1:2">
-      <c r="A128" s="5"/>
+      <c r="C127" s="5"/>
+    </row>
+    <row r="128" spans="2:3">
       <c r="B128" s="5"/>
-    </row>
-    <row r="129" spans="1:2">
-      <c r="A129" s="5"/>
+      <c r="C128" s="5"/>
+    </row>
+    <row r="129" spans="2:3">
       <c r="B129" s="5"/>
-    </row>
-    <row r="130" spans="1:2">
-      <c r="A130" s="5"/>
+      <c r="C129" s="5"/>
+    </row>
+    <row r="130" spans="2:3">
       <c r="B130" s="5"/>
-    </row>
-    <row r="131" spans="1:2">
-      <c r="A131" s="5"/>
+      <c r="C130" s="5"/>
+    </row>
+    <row r="131" spans="2:3">
       <c r="B131" s="5"/>
-    </row>
-    <row r="132" spans="1:2">
-      <c r="A132" s="5"/>
+      <c r="C131" s="5"/>
+    </row>
+    <row r="132" spans="2:3">
       <c r="B132" s="5"/>
-    </row>
-    <row r="133" spans="1:2">
-      <c r="A133" s="5"/>
+      <c r="C132" s="5"/>
+    </row>
+    <row r="133" spans="2:3">
       <c r="B133" s="5"/>
-    </row>
-    <row r="134" spans="1:2">
-      <c r="A134" s="5"/>
+      <c r="C133" s="5"/>
+    </row>
+    <row r="134" spans="2:3">
       <c r="B134" s="5"/>
-    </row>
-    <row r="135" spans="1:2">
-      <c r="A135" s="5"/>
+      <c r="C134" s="5"/>
+    </row>
+    <row r="135" spans="2:3">
       <c r="B135" s="5"/>
-    </row>
-    <row r="136" spans="1:2">
-      <c r="A136" s="5"/>
+      <c r="C135" s="5"/>
+    </row>
+    <row r="136" spans="2:3">
       <c r="B136" s="5"/>
-    </row>
-    <row r="137" spans="1:2">
-      <c r="A137" s="5"/>
+      <c r="C136" s="5"/>
+    </row>
+    <row r="137" spans="2:3">
       <c r="B137" s="5"/>
-    </row>
-    <row r="138" spans="1:2">
-      <c r="A138" s="5"/>
+      <c r="C137" s="5"/>
+    </row>
+    <row r="138" spans="2:3">
       <c r="B138" s="5"/>
-    </row>
-    <row r="139" spans="1:2">
-      <c r="A139" s="5"/>
+      <c r="C138" s="5"/>
+    </row>
+    <row r="139" spans="2:3">
       <c r="B139" s="5"/>
-    </row>
-    <row r="140" spans="1:2">
-      <c r="A140" s="5"/>
+      <c r="C139" s="5"/>
+    </row>
+    <row r="140" spans="2:3">
       <c r="B140" s="5"/>
-    </row>
-    <row r="141" spans="1:2">
-      <c r="A141" s="5"/>
+      <c r="C140" s="5"/>
+    </row>
+    <row r="141" spans="2:3">
       <c r="B141" s="5"/>
-    </row>
-    <row r="142" spans="1:2">
-      <c r="A142" s="5"/>
+      <c r="C141" s="5"/>
+    </row>
+    <row r="142" spans="2:3">
       <c r="B142" s="5"/>
-    </row>
-    <row r="143" spans="1:2">
-      <c r="A143" s="5"/>
+      <c r="C142" s="5"/>
+    </row>
+    <row r="143" spans="2:3">
       <c r="B143" s="5"/>
-    </row>
-    <row r="144" spans="1:2">
-      <c r="A144" s="5"/>
+      <c r="C143" s="5"/>
+    </row>
+    <row r="144" spans="2:3">
       <c r="B144" s="5"/>
-    </row>
-    <row r="145" spans="1:2">
-      <c r="A145" s="5"/>
+      <c r="C144" s="5"/>
+    </row>
+    <row r="145" spans="2:3">
       <c r="B145" s="5"/>
-    </row>
-    <row r="146" spans="1:2">
-      <c r="A146" s="5"/>
+      <c r="C145" s="5"/>
+    </row>
+    <row r="146" spans="2:3">
       <c r="B146" s="5"/>
-    </row>
-    <row r="147" spans="1:2">
-      <c r="A147" s="5"/>
+      <c r="C146" s="5"/>
+    </row>
+    <row r="147" spans="2:3">
       <c r="B147" s="5"/>
-    </row>
-    <row r="148" spans="1:2">
-      <c r="A148" s="5"/>
+      <c r="C147" s="5"/>
+    </row>
+    <row r="148" spans="2:3">
       <c r="B148" s="5"/>
-    </row>
-    <row r="149" spans="1:2">
-      <c r="A149" s="5"/>
+      <c r="C148" s="5"/>
+    </row>
+    <row r="149" spans="2:3">
       <c r="B149" s="5"/>
-    </row>
-    <row r="150" spans="1:2">
-      <c r="A150" s="5"/>
+      <c r="C149" s="5"/>
+    </row>
+    <row r="150" spans="2:3">
       <c r="B150" s="5"/>
-    </row>
-    <row r="151" spans="1:2">
-      <c r="A151" s="5"/>
+      <c r="C150" s="5"/>
+    </row>
+    <row r="151" spans="2:3">
       <c r="B151" s="5"/>
-    </row>
-    <row r="152" spans="1:2">
-      <c r="A152" s="5"/>
+      <c r="C151" s="5"/>
+    </row>
+    <row r="152" spans="2:3">
       <c r="B152" s="5"/>
-    </row>
-    <row r="153" spans="1:2">
-      <c r="A153" s="5"/>
+      <c r="C152" s="5"/>
+    </row>
+    <row r="153" spans="2:3">
       <c r="B153" s="5"/>
-    </row>
-    <row r="154" spans="1:2">
-      <c r="A154" s="5"/>
+      <c r="C153" s="5"/>
+    </row>
+    <row r="154" spans="2:3">
       <c r="B154" s="5"/>
-    </row>
-    <row r="155" spans="1:2">
-      <c r="A155" s="5"/>
+      <c r="C154" s="5"/>
+    </row>
+    <row r="155" spans="2:3">
       <c r="B155" s="5"/>
-    </row>
-    <row r="156" spans="1:2">
-      <c r="A156" s="5"/>
+      <c r="C155" s="5"/>
+    </row>
+    <row r="156" spans="2:3">
       <c r="B156" s="5"/>
-    </row>
-    <row r="157" spans="1:2">
-      <c r="A157" s="5"/>
-      <c r="B157" s="5"/>
+      <c r="C156" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>